<commit_message>
Edited and added file
</commit_message>
<xml_diff>
--- a/responses.xlsx
+++ b/responses.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>Timestamp</t>
   </si>
@@ -27,6 +27,15 @@
   </si>
   <si>
     <t>2025-08-05T06:10:41.492Z</t>
+  </si>
+  <si>
+    <t>2025-08-06T01:53:22.718Z</t>
+  </si>
+  <si>
+    <t>2025-08-06T01:54:07.017Z</t>
+  </si>
+  <si>
+    <t>2025-08-06T01:54:08.635Z</t>
   </si>
 </sst>
 </file>
@@ -438,7 +447,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -449,6 +458,30 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>